<commit_message>
Add new footprints, change project template structure
</commit_message>
<xml_diff>
--- a/__Project__/docs/__Project__.xlsx
+++ b/__Project__/docs/__Project__.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E52E0A8-05E7-4BD4-BD56-2442D95214CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEFB041-3649-4E61-9F82-B3BF5A271680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28470" yWindow="315" windowWidth="7185" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -1215,29 +1215,29 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1551,7 +1551,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1569,10 +1569,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="48.6" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="73"/>
       <c r="C1" s="43"/>
       <c r="D1" s="44"/>
       <c r="E1" s="43"/>
@@ -1581,7 +1581,7 @@
       <c r="H1" s="26"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="2" spans="1:11" s="18" customFormat="1" ht="15">
       <c r="A2" s="74" t="s">
         <v>40</v>
       </c>
@@ -1594,25 +1594,25 @@
       <c r="F2" s="67"/>
       <c r="G2" s="67"/>
     </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="3" spans="1:11" s="18" customFormat="1" ht="15">
       <c r="A3" s="74" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="74"/>
       <c r="C3" s="68">
         <f ca="1">TODAY()</f>
-        <v>45157</v>
+        <v>45169</v>
       </c>
       <c r="D3" s="65"/>
       <c r="E3" s="65"/>
       <c r="F3" s="65"/>
       <c r="G3" s="65"/>
     </row>
-    <row r="4" spans="1:11" s="18" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A4" s="76" t="s">
+    <row r="4" spans="1:11" s="18" customFormat="1" ht="15">
+      <c r="A4" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="76"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="45" t="s">
         <v>37</v>
       </c>
@@ -1621,11 +1621,11 @@
       <c r="F4" s="45"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:11" s="18" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A5" s="76" t="s">
+    <row r="5" spans="1:11" s="18" customFormat="1" ht="15">
+      <c r="A5" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="76"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="45" t="s">
         <v>37</v>
       </c>
@@ -2181,31 +2181,31 @@
     </row>
     <row r="47" spans="1:11" s="42" customFormat="1" ht="14.25" customHeight="1">
       <c r="A47" s="69"/>
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
       <c r="E47" s="25"/>
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" s="39" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A48" s="79"/>
-      <c r="B48" s="73" t="s">
+      <c r="A48" s="72"/>
+      <c r="B48" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
       <c r="E48" s="38"/>
       <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="15">
       <c r="A49" s="70"/>
-      <c r="B49" s="72" t="s">
+      <c r="B49" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="72"/>
-      <c r="D49" s="72"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
       <c r="E49" s="6"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="50" spans="1:8" ht="15">
       <c r="A50" s="71"/>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
       <c r="E50" s="6"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2250,15 +2250,15 @@
   </sheetData>
   <sheetProtection formatCells="0" insertRows="0" deleteRows="0" sort="0"/>
   <mergeCells count="9">
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2287,27 +2287,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="48.6" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="78"/>
       <c r="C1" s="43"/>
       <c r="D1" s="44"/>
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" s="18" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A2" s="78" t="str">
+      <c r="A2" s="79" t="str">
         <f>Stückliste!A2</f>
         <v xml:space="preserve">Bezeichnung / Name: </v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>45157</v>
+        <v>45169</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="18" customFormat="1" ht="19.899999999999999" customHeight="1">
@@ -2673,11 +2673,11 @@
       <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" s="17" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A2" s="78" t="str">
+      <c r="A2" s="79" t="str">
         <f>Stückliste!A2</f>
         <v xml:space="preserve">Bezeichnung / Name: </v>
       </c>
-      <c r="B2" s="78"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="30"/>
       <c r="D2" s="27">
         <f>Stückliste!H2</f>

</xml_diff>